<commit_message>
Branch Finaneceiro - Primeiro commit
</commit_message>
<xml_diff>
--- a/1_carga_horaria_detalhada.xlsx
+++ b/1_carga_horaria_detalhada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F65"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,12 +483,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>PAM26_PRO_12</t>
+          <t>PAM_PRO_12</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -513,12 +513,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>PAM26_PRO_13</t>
+          <t>PAM_PRO_13</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -663,12 +663,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>PAM26_PRO_12</t>
+          <t>PAM_PRO_12</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -693,12 +693,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>PAM26_PRO_13</t>
+          <t>PAM_PRO_13</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -713,7 +713,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -843,12 +843,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>PAM26_PRO_12</t>
+          <t>PAM_PRO_12</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -863,7 +863,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -873,12 +873,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>PAM26_PRO_13</t>
+          <t>PAM_PRO_13</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -888,12 +888,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -903,12 +903,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DD1_PRO_0</t>
+          <t>PAM_PRO_8</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -918,12 +918,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -933,12 +933,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DD1_PRO_2</t>
+          <t>PAM_PRO_9</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -948,12 +948,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -963,12 +963,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>DD1_PRO_3</t>
+          <t>PAM_PRO_11</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -978,12 +978,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -993,12 +993,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>DD1_PRO_6</t>
+          <t>PAM_PRO_16</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1008,12 +1008,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1023,12 +1023,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>PAM26_PRO_12</t>
+          <t>DD1_PRO_1</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1038,12 +1038,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PROG_1</t>
+          <t>PROG_2</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1053,12 +1053,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>PAM26_PRO_13</t>
+          <t>DD1_PRO_5</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1083,12 +1083,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>PAM26_PRO_8</t>
+          <t>PAM_PRO_8</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1113,12 +1113,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>PAM26_PRO_9</t>
+          <t>PAM_PRO_9</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1143,12 +1143,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>PAM26_PRO_11</t>
+          <t>PAM_PRO_11</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>PAM26_PRO_16</t>
+          <t>PAM_PRO_16</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1263,12 +1263,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>PAM26_PRO_8</t>
+          <t>PAM_PRO_8</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1293,12 +1293,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>PAM26_PRO_9</t>
+          <t>PAM_PRO_9</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>PAM26_PRO_11</t>
+          <t>PAM_PRO_11</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fev/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1353,12 +1353,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>PAM26_PRO_16</t>
+          <t>PAM_PRO_16</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1368,12 +1368,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1383,12 +1383,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>DD1_PRO_1</t>
+          <t>PAM_PRO_10</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1398,12 +1398,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1413,12 +1413,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>DD1_PRO_5</t>
+          <t>PAM_PRO_14</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1428,12 +1428,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1443,12 +1443,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>PAM26_PRO_8</t>
+          <t>PAM_PRO_15</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1458,12 +1458,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Abr/26</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1473,12 +1473,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>PAM26_PRO_9</t>
+          <t>PAM_PRO_17</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -1488,12 +1488,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1503,12 +1503,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>PAM26_PRO_11</t>
+          <t>DD1_PRO_4</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -1518,12 +1518,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Jan/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1533,12 +1533,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>PAM26_PRO_16</t>
+          <t>DD1_PRO_7</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -1548,12 +1548,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1563,12 +1563,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>DD1_PRO_1</t>
+          <t>PAM_PRO_10</t>
         </is>
       </c>
       <c r="F38" t="n">
@@ -1578,12 +1578,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1593,12 +1593,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>DD1</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>DD1_PRO_5</t>
+          <t>PAM_PRO_14</t>
         </is>
       </c>
       <c r="F39" t="n">
@@ -1608,12 +1608,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>PAM26_PRO_8</t>
+          <t>PAM_PRO_15</t>
         </is>
       </c>
       <c r="F40" t="n">
@@ -1638,12 +1638,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Mar/26</t>
+          <t>Fev/26</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1653,12 +1653,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>PAM26_PRO_9</t>
+          <t>PAM_PRO_17</t>
         </is>
       </c>
       <c r="F41" t="n">
@@ -1668,7 +1668,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1683,12 +1683,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>PAM26_PRO_11</t>
+          <t>DD1_PRO_4</t>
         </is>
       </c>
       <c r="F42" t="n">
@@ -1698,7 +1698,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>PROG_2</t>
+          <t>PROG_3</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1713,12 +1713,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>DD1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>PAM26_PRO_16</t>
+          <t>DD1_PRO_7</t>
         </is>
       </c>
       <c r="F43" t="n">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1743,12 +1743,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>PAM26_PRO_10</t>
+          <t>PAM_PRO_10</t>
         </is>
       </c>
       <c r="F44" t="n">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1773,12 +1773,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>PAM26_PRO_14</t>
+          <t>PAM_PRO_14</t>
         </is>
       </c>
       <c r="F45" t="n">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1803,12 +1803,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>PAM26_PRO_15</t>
+          <t>PAM_PRO_15</t>
         </is>
       </c>
       <c r="F46" t="n">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Abr/26</t>
+          <t>Mar/26</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1833,555 +1833,15 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>PAM26</t>
+          <t>PAM</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>PAM26_PRO_17</t>
+          <t>PAM_PRO_17</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>DD1_PRO_4</t>
-        </is>
-      </c>
-      <c r="F48" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>DD1_PRO_7</t>
-        </is>
-      </c>
-      <c r="F49" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_10</t>
-        </is>
-      </c>
-      <c r="F50" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_14</t>
-        </is>
-      </c>
-      <c r="F51" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_15</t>
-        </is>
-      </c>
-      <c r="F52" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Fev/26</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_17</t>
-        </is>
-      </c>
-      <c r="F53" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>DD1_PRO_4</t>
-        </is>
-      </c>
-      <c r="F54" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>DD1_PRO_7</t>
-        </is>
-      </c>
-      <c r="F55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_10</t>
-        </is>
-      </c>
-      <c r="F56" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_14</t>
-        </is>
-      </c>
-      <c r="F57" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_15</t>
-        </is>
-      </c>
-      <c r="F58" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Jan/26</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_17</t>
-        </is>
-      </c>
-      <c r="F59" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>DD1_PRO_4</t>
-        </is>
-      </c>
-      <c r="F60" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>DD1</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>DD1_PRO_7</t>
-        </is>
-      </c>
-      <c r="F61" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_10</t>
-        </is>
-      </c>
-      <c r="F62" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_14</t>
-        </is>
-      </c>
-      <c r="F63" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_15</t>
-        </is>
-      </c>
-      <c r="F64" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>PROG_3</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Mar/26</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>PROG</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>PAM26</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>PAM26_PRO_17</t>
-        </is>
-      </c>
-      <c r="F65" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>